<commit_message>
9th Stab- Cosmetic Changes
</commit_message>
<xml_diff>
--- a/Reports/MarketBeatRank/TanzyGrowth/CDXS.xlsx
+++ b/Reports/MarketBeatRank/TanzyGrowth/CDXS.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="35">
   <si>
     <t>Jun_10</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>6/13/2018,Downgrades,Strong-Buy -&gt; Buy,</t>
+  </si>
+  <si>
+    <t>Jun_15</t>
+  </si>
+  <si>
+    <t>Jun_17</t>
   </si>
 </sst>
 </file>
@@ -170,7 +176,7 @@
   <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="true" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf applyFill="true" borderId="0" fillId="5" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -183,14 +189,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="8.0" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="8.0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>0</v>
       </c>
     </row>
@@ -204,6 +218,12 @@
       <c r="C2" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -215,6 +235,12 @@
       <c r="C3" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -226,6 +252,12 @@
       <c r="C4" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
@@ -237,6 +269,12 @@
       <c r="C5" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -248,6 +286,12 @@
       <c r="C6" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
@@ -259,6 +303,12 @@
       <c r="C7" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
@@ -270,6 +320,12 @@
       <c r="C8" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
@@ -281,6 +337,12 @@
       <c r="C9" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
@@ -292,6 +354,12 @@
       <c r="C10" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
@@ -303,6 +371,12 @@
       <c r="C11" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
@@ -314,6 +388,12 @@
       <c r="C12" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
@@ -322,7 +402,13 @@
       <c r="B13" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -336,6 +422,12 @@
       <c r="C14" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
@@ -347,6 +439,12 @@
       <c r="C15" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
@@ -358,6 +456,12 @@
       <c r="C16" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
@@ -369,6 +473,12 @@
       <c r="C17" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
@@ -380,6 +490,12 @@
       <c r="C18" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
@@ -391,6 +507,12 @@
       <c r="C19" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
@@ -402,6 +524,12 @@
       <c r="C20" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
@@ -413,15 +541,27 @@
       <c r="C21" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="E22" s="0" t="s">
         <v>2</v>
       </c>
     </row>
@@ -435,6 +575,12 @@
       <c r="C23" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
@@ -446,6 +592,12 @@
       <c r="C24" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
@@ -457,6 +609,12 @@
       <c r="C25" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
@@ -466,6 +624,12 @@
         <v>2</v>
       </c>
       <c r="C26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" s="0" t="s">
         <v>27</v>
       </c>
     </row>
@@ -477,6 +641,12 @@
         <v>2</v>
       </c>
       <c r="C27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" s="0" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
10Th - MB for single stock and added new group
</commit_message>
<xml_diff>
--- a/Reports/MarketBeatRank/TanzyGrowth/CDXS.xlsx
+++ b/Reports/MarketBeatRank/TanzyGrowth/CDXS.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1370" uniqueCount="39">
   <si>
     <t>Jun_10</t>
   </si>
@@ -117,6 +117,18 @@
   </si>
   <si>
     <t>Jun_17</t>
+  </si>
+  <si>
+    <t>Jun_26</t>
+  </si>
+  <si>
+    <t>Benchmark</t>
+  </si>
+  <si>
+    <t>Evercore ISI</t>
+  </si>
+  <si>
+    <t>Jun_27</t>
   </si>
 </sst>
 </file>
@@ -173,10 +185,94 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="87">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="true" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="true" borderId="0" fillId="5" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -191,20 +287,32 @@
   <cols>
     <col min="3" max="3" customWidth="true" width="8.0" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="8.0" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="8.0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>0</v>
       </c>
     </row>
@@ -224,6 +332,15 @@
       <c r="E2" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -241,6 +358,15 @@
       <c r="E3" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -258,6 +384,15 @@
       <c r="E4" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
@@ -275,6 +410,15 @@
       <c r="E5" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -292,6 +436,15 @@
       <c r="E6" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
@@ -309,6 +462,15 @@
       <c r="E7" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
@@ -326,6 +488,15 @@
       <c r="E8" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
@@ -343,6 +514,15 @@
       <c r="E9" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
@@ -360,6 +540,15 @@
       <c r="E10" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
@@ -377,6 +566,15 @@
       <c r="E11" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
@@ -394,6 +592,15 @@
       <c r="E12" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
@@ -408,7 +615,16 @@
       <c r="D13" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -428,6 +644,15 @@
       <c r="E14" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
@@ -445,6 +670,15 @@
       <c r="E15" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
@@ -462,6 +696,15 @@
       <c r="E16" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
@@ -479,6 +722,15 @@
       <c r="E17" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
@@ -496,6 +748,15 @@
       <c r="E18" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
@@ -513,6 +774,15 @@
       <c r="E19" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
@@ -530,6 +800,15 @@
       <c r="E20" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
@@ -547,6 +826,15 @@
       <c r="E21" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
@@ -558,10 +846,19 @@
       <c r="C22" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E22" s="0" t="s">
+      <c r="H22" s="0" t="s">
         <v>2</v>
       </c>
     </row>
@@ -581,6 +878,15 @@
       <c r="E23" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
@@ -598,6 +904,15 @@
       <c r="E24" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
@@ -615,6 +930,15 @@
       <c r="E25" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
@@ -630,6 +954,15 @@
         <v>2</v>
       </c>
       <c r="E26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="H26" s="0" t="s">
         <v>27</v>
       </c>
     </row>
@@ -647,6 +980,43 @@
         <v>2</v>
       </c>
       <c r="E27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="0" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>